<commit_message>
change domain remove whitespace and umlaute
</commit_message>
<xml_diff>
--- a/python_setup/240617.xlsx
+++ b/python_setup/240617.xlsx
@@ -501,7 +501,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>www.alour.web.bbq</t>
+          <t>www.wasim-web.bbq</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>www.bouzir.web.bbq</t>
+          <t>www.amaanilinda-web.bbq</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -545,7 +545,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>www.bublyk.web.bbq</t>
+          <t>www.serhii-web.bbq</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>www.ioschpa.web.bbq</t>
+          <t>www.elina-web.bbq</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -589,7 +589,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>www.jalbout.web.bbq</t>
+          <t>www.mohammed-web.bbq</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>www.likhareva.web.bbq</t>
+          <t>www.marina-web.bbq</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>www.rattab.web.bbq</t>
+          <t>www.ilyas-web.bbq</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -655,7 +655,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>www.stolzenburg.web.bbq</t>
+          <t>www.david-web.bbq</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -677,7 +677,7 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>www.trautwein.web.bbq</t>
+          <t>www.thomas-web.bbq</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -699,7 +699,7 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>www.el-haj.web.bbq</t>
+          <t>www.hadi-web.bbq</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>www.güneri.web.bbq</t>
+          <t>www.enes-web.bbq</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>www.pathak.web.bbq</t>
+          <t>www.jitender-web.bbq</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -765,7 +765,7 @@
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>www.elitas.web.bbq</t>
+          <t>www.cetin-web.bbq</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>www.effati khurram .web.bbq</t>
+          <t>www.ehsan-web.bbq</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>www.melanie.web.bbq</t>
+          <t>www.melzer-web.bbq</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>www.mischell.web.bbq</t>
+          <t>www.bogenberg-web.bbq</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">

</xml_diff>